<commit_message>
inline keyboard at start added
</commit_message>
<xml_diff>
--- a/applies.xlsx
+++ b/applies.xlsx
@@ -458,22 +458,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sdflkj</t>
+          <t>dsfdsf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sdfjl</t>
+          <t>vbfvb</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>380664606978</t>
+          <t>+380664606978</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>04/12/2023 17:31:40</t>
+          <t>11/12/2023 18:36:45</t>
         </is>
       </c>
     </row>

</xml_diff>